<commit_message>
Update homeless population by Race.xlsx
</commit_message>
<xml_diff>
--- a/Data/homeless population by Race.xlsx
+++ b/Data/homeless population by Race.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c1abe71445d0fcf/Documents/Data Scientist Program/Final Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c1abe71445d0fcf/Documents/GitHub/Homelessness-Final-Group-Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F76F2747-7CA0-404D-B689-A1725BD725F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{F76F2747-7CA0-404D-B689-A1725BD725F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6AE072C-EC34-4B42-B276-F8C136C3AA78}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{71AC762F-AA51-4FD2-82FC-828826313791}"/>
   </bookViews>
@@ -37,25 +37,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t xml:space="preserve">        Multiple races </t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Pacific Islander </t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Native American </t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Asian </t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Black </t>
-  </si>
-  <si>
-    <t xml:space="preserve">        White </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    By race</t>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Native American</t>
+  </si>
+  <si>
+    <t>Pacific Islander</t>
+  </si>
+  <si>
+    <t>Multiple Races</t>
+  </si>
+  <si>
+    <t>Years</t>
   </si>
 </sst>
 </file>
@@ -91,8 +91,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,177 +410,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AAE2807-F450-4A91-B910-9F15A33F63E0}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>2015</v>
       </c>
-      <c r="C1">
+      <c r="B2" s="1">
+        <v>273746</v>
+      </c>
+      <c r="C2" s="1">
+        <v>227937</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6074</v>
+      </c>
+      <c r="E2" s="1">
+        <v>15136</v>
+      </c>
+      <c r="F2" s="1">
+        <v>8827</v>
+      </c>
+      <c r="G2" s="1">
+        <v>32988</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2016</v>
       </c>
-      <c r="D1">
+      <c r="B3" s="1">
+        <v>265660</v>
+      </c>
+      <c r="C3" s="1">
+        <v>215177</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5603</v>
+      </c>
+      <c r="E3" s="1">
+        <v>15229</v>
+      </c>
+      <c r="F3" s="1">
+        <v>8734</v>
+      </c>
+      <c r="G3" s="1">
+        <v>39525</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2017</v>
       </c>
-      <c r="E1">
+      <c r="B4" s="1">
+        <v>259675</v>
+      </c>
+      <c r="C4" s="1">
+        <v>223690</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6700</v>
+      </c>
+      <c r="E4" s="1">
+        <v>16741</v>
+      </c>
+      <c r="F4" s="1">
+        <v>8515</v>
+      </c>
+      <c r="G4" s="1">
+        <v>35675</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>2018</v>
       </c>
-      <c r="F1">
+      <c r="B5" s="1">
+        <v>270568</v>
+      </c>
+      <c r="C5" s="1">
+        <v>219809</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6643</v>
+      </c>
+      <c r="E5" s="1">
+        <v>15414</v>
+      </c>
+      <c r="F5" s="1">
+        <v>8039</v>
+      </c>
+      <c r="G5" s="1">
+        <v>32357</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>2019</v>
       </c>
-      <c r="G1">
+      <c r="B6" s="1">
+        <v>270607</v>
+      </c>
+      <c r="C6" s="1">
+        <v>225735</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7228</v>
+      </c>
+      <c r="E6" s="1">
+        <v>17966</v>
+      </c>
+      <c r="F6" s="1">
+        <v>9311</v>
+      </c>
+      <c r="G6" s="1">
+        <v>36868</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>2020</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>273746</v>
-      </c>
-      <c r="C2">
-        <v>265660</v>
-      </c>
-      <c r="D2">
-        <v>259675</v>
-      </c>
-      <c r="E2">
-        <v>270568</v>
-      </c>
-      <c r="F2">
-        <v>270607</v>
-      </c>
-      <c r="G2">
+      <c r="B7" s="1">
         <v>280612</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>227937</v>
-      </c>
-      <c r="C3">
-        <v>215177</v>
-      </c>
-      <c r="D3">
-        <v>223690</v>
-      </c>
-      <c r="E3">
-        <v>219809</v>
-      </c>
-      <c r="F3">
-        <v>225735</v>
-      </c>
-      <c r="G3">
+      <c r="C7" s="1">
         <v>228796</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>6074</v>
-      </c>
-      <c r="C4">
-        <v>5603</v>
-      </c>
-      <c r="D4">
-        <v>6700</v>
-      </c>
-      <c r="E4">
-        <v>6643</v>
-      </c>
-      <c r="F4">
-        <v>7228</v>
-      </c>
-      <c r="G4">
+      <c r="D7" s="1">
         <v>7638</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>15136</v>
-      </c>
-      <c r="C5">
-        <v>15229</v>
-      </c>
-      <c r="D5">
-        <v>16741</v>
-      </c>
-      <c r="E5">
-        <v>15414</v>
-      </c>
-      <c r="F5">
-        <v>17966</v>
-      </c>
-      <c r="G5">
+      <c r="E7" s="1">
         <v>18935</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>8827</v>
-      </c>
-      <c r="C6">
-        <v>8734</v>
-      </c>
-      <c r="D6">
-        <v>8515</v>
-      </c>
-      <c r="E6">
-        <v>8039</v>
-      </c>
-      <c r="F6">
-        <v>9311</v>
-      </c>
-      <c r="G6">
+      <c r="F7" s="1">
         <v>8794</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>32988</v>
-      </c>
-      <c r="C7">
-        <v>39525</v>
-      </c>
-      <c r="D7">
-        <v>35675</v>
-      </c>
-      <c r="E7">
-        <v>32357</v>
-      </c>
-      <c r="F7">
-        <v>36868</v>
-      </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>35680</v>
       </c>
+      <c r="H7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>